<commit_message>
Added return value for statistics
</commit_message>
<xml_diff>
--- a/template/Tour create template.xlsx
+++ b/template/Tour create template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF97F373-1316-4ECD-80A8-CBC5E3249780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606B4875-B214-4FE4-AEAC-5E3C882F0A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2712" yWindow="1032" windowWidth="18708" windowHeight="11328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Tour Name</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Route</t>
-  </si>
-  <si>
-    <t>Route bla bla</t>
   </si>
   <si>
     <t>Example
@@ -55,6 +52,12 @@
   </si>
   <si>
     <t>Note: Scanning from number 1 -&gt; 10. Please fill out the whole row to create a tour</t>
+  </si>
+  <si>
+    <t>Ticket Description</t>
+  </si>
+  <si>
+    <t>Route biển</t>
   </si>
 </sst>
 </file>
@@ -535,7 +538,7 @@
   <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -554,7 +557,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.8" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -720,10 +723,10 @@
     </row>
     <row r="14" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>2</v>
@@ -741,7 +744,7 @@
         <v>0.27083333333212067</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -764,6 +767,9 @@
     </row>
     <row r="16" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing Tour create template
</commit_message>
<xml_diff>
--- a/template/Tour create template.xlsx
+++ b/template/Tour create template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606B4875-B214-4FE4-AEAC-5E3C882F0A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB748F12-C4F5-4A5A-AC46-F80A4243E0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Tour Name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Route biển</t>
+  </si>
+  <si>
+    <t>Route available</t>
   </si>
 </sst>
 </file>
@@ -535,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -765,11 +768,19 @@
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
     </row>
+    <row r="15" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>